<commit_message>
Verified Peripheral and Motor power controllers
</commit_message>
<xml_diff>
--- a/Electrical/MotorPowerControl/BOM-MotorPowerControl.xlsx
+++ b/Electrical/MotorPowerControl/BOM-MotorPowerControl.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jklei\Desktop\Projects\igvc_hardware_2020\Electrical\MotorPowerControl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3809D5FB-FAB4-4E69-AB08-81C6F6BA1448}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86C7B51D-2E73-44E8-9DB4-E795ABA440F3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2106" yWindow="2106" windowWidth="17280" windowHeight="8994" xr2:uid="{0BA19F0C-F245-4227-997C-7F95E7CEF7C8}"/>
+    <workbookView xWindow="2442" yWindow="2442" windowWidth="17280" windowHeight="8994" xr2:uid="{0BA19F0C-F245-4227-997C-7F95E7CEF7C8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -45,9 +45,6 @@
     <t>https://www.mouser.com/ProductDetail/Littelfuse/17861640002?qs=sGAEpiMZZMtRmoYvq3OwzPmB3P758op4Wz%252BhK9S1jNg%3D</t>
   </si>
   <si>
-    <t>Heatshrink</t>
-  </si>
-  <si>
     <t>CUI</t>
   </si>
   <si>
@@ -76,6 +73,9 @@
   </si>
   <si>
     <t>Link</t>
+  </si>
+  <si>
+    <t>Heatsink</t>
   </si>
 </sst>
 </file>
@@ -467,7 +467,7 @@
   <dimension ref="B2:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:H2"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -480,25 +480,25 @@
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>13</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.55000000000000004">
@@ -527,13 +527,13 @@
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>6</v>
       </c>
       <c r="E4" s="2">
         <v>0.57999999999999996</v>
@@ -545,13 +545,14 @@
         <f>F4*E4</f>
         <v>1.1599999999999999</v>
       </c>
-      <c r="H4" t="s">
-        <v>7</v>
+      <c r="H4" s="4" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="H3" r:id="rId1" xr:uid="{DF0FBCF9-5F05-4F97-89CE-510F20F6359A}"/>
+    <hyperlink ref="H4" r:id="rId2" xr:uid="{C7B9B0B0-CF39-4EE3-99F5-2AC71897E3E8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>